<commit_message>
Change of v3 in machine cost
</commit_message>
<xml_diff>
--- a/data/cost/PLA_cost_table.xlsx
+++ b/data/cost/PLA_cost_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EEF65A-C3F2-ED44-98A8-9FE59B85B53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D77053-577E-6646-B0B2-39859ADBB72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="17980" windowHeight="18240" activeTab="3" xr2:uid="{9E23791E-A9D1-B24D-9D6E-42C1F180DBE7}"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="17980" windowHeight="18240" activeTab="2" xr2:uid="{9E23791E-A9D1-B24D-9D6E-42C1F180DBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="shredding" sheetId="1" r:id="rId1"/>
@@ -23,23 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="24">
-  <si>
-    <t>machine_purchase cost_[€]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="22">
   <si>
     <t>machine_purchase_cost_[€]</t>
   </si>
@@ -99,9 +88,6 @@
   </si>
   <si>
     <t>machine_life_span_[y]</t>
-  </si>
-  <si>
-    <t>cost_of_spare_parts_[€]</t>
   </si>
   <si>
     <t>operational_rate_time_[€/y]</t>
@@ -472,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CECAF4-10EE-7547-8F9A-E08E88E519F7}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="116" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -500,28 +486,28 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -529,58 +515,58 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
-        <v>17</v>
-      </c>
       <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -655,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14329C3B-818D-974A-839B-1CDF92A21CC9}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="G1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,28 +669,28 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -712,58 +698,58 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
         <v>21</v>
-      </c>
-      <c r="O2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -838,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F903924-2D1B-F649-8D6E-329FE2160CED}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -866,28 +852,28 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -898,55 +884,55 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
-        <v>17</v>
-      </c>
       <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -1021,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C261B8B2-5703-4A47-9A2B-A87AD92FEE9B}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+    <sheetView zoomScale="86" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1049,28 +1035,28 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1079,58 +1065,58 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
-        <v>17</v>
-      </c>
       <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
       <c r="R2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>